<commit_message>
added code for generating subsets, renaming column names and recoding variables
</commit_message>
<xml_diff>
--- a/01_20231123_srlwq_deu.xlsx
+++ b/01_20231123_srlwq_deu.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\workpl_srl_thesis_phhd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D4A807-C447-4A7A-9023-BD2D61323B20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{732A300C-A7D8-400B-820C-A3937781F821}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F44CDD34-D03A-47D1-A95E-AC299A1E3140}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8892" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8968" uniqueCount="239">
   <si>
     <t>ID</t>
   </si>
@@ -1106,8 +1107,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB9B35E0-FEC3-4173-AD93-E986F8E245B3}">
   <dimension ref="A1:BX117"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="BN1" workbookViewId="0">
+      <selection sqref="A1:BX1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -28025,4 +28026,399 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{07297A7D-B9D4-41AB-9F6A-786D78C31581}">
+  <dimension ref="A1:A76"/>
+  <sheetViews>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection sqref="A1:A76"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>